<commit_message>
Edit station linked with uploaded excel
</commit_message>
<xml_diff>
--- a/Green_Schedule.xlsx
+++ b/Green_Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasse\Desktop\ECE1140\Team_X_ECE_1140\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCE21C7-B943-404C-BCFB-3490C0487441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0A0F46-E692-4086-97EF-4C18672E9DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16050" yWindow="390" windowWidth="11340" windowHeight="14160" xr2:uid="{2B5606EC-EDD7-49E1-9BF7-E3A623A115DD}"/>
+    <workbookView xWindow="16212" yWindow="0" windowWidth="4572" windowHeight="12360" xr2:uid="{2B5606EC-EDD7-49E1-9BF7-E3A623A115DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -464,111 +464,111 @@
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>44901.666666666664</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>44902.636805555558</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Fixed Maintenance mode crashing
</commit_message>
<xml_diff>
--- a/Green_Schedule.xlsx
+++ b/Green_Schedule.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasse\Desktop\ECE1140\Team_X_ECE_1140\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0A0F46-E692-4086-97EF-4C18672E9DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1952D754-7EFA-4EDA-9BEA-7F055F56E0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16212" yWindow="0" windowWidth="4572" windowHeight="12360" xr2:uid="{2B5606EC-EDD7-49E1-9BF7-E3A623A115DD}"/>
+    <workbookView xWindow="3855" yWindow="1545" windowWidth="4170" windowHeight="11325" xr2:uid="{2B5606EC-EDD7-49E1-9BF7-E3A623A115DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -92,7 +92,7 @@
     <t>OVERBROOK I</t>
   </si>
   <si>
-    <t>Time, Line, and Stations</t>
+    <t>Time and Stations</t>
   </si>
 </sst>
 </file>
@@ -464,111 +464,111 @@
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44902.636805555558</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>